<commit_message>
Aguscalientes, Guanajuato, Queretaro e Hidalgo
</commit_message>
<xml_diff>
--- a/Resources/data/COMPILADO DE  ENTIDADES FEDERATIVAS.xlsx
+++ b/Resources/data/COMPILADO DE  ENTIDADES FEDERATIVAS.xlsx
@@ -826,7 +826,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -835,19 +835,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1168,139 +1156,139 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1313,46 +1301,41 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1688,10 +1671,10 @@
   <sheetPr/>
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1707,40 +1690,40 @@
   </cols>
   <sheetData>
     <row r="1" ht="71.25" spans="1:12">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1757,10 +1740,10 @@
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -1775,68 +1758,68 @@
       <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A3" s="2" t="s">
+    <row r="3" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="2" t="s">
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" s="3" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A4" s="3" t="s">
+    <row r="4" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="16" t="s">
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1844,19 +1827,19 @@
       <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="14" t="s">
         <v>35</v>
       </c>
       <c r="G5" t="s">
@@ -1871,39 +1854,39 @@
       <c r="J5" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" s="2" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A6" s="2" t="s">
+    <row r="6" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="2" t="s">
+      <c r="G6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1920,10 +1903,10 @@
       <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>45</v>
       </c>
       <c r="G7" t="s">
@@ -1938,10 +1921,10 @@
       <c r="J7" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="4" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1958,7 +1941,7 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F8" t="s">
@@ -1976,86 +1959,86 @@
       <c r="J8" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" s="2" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A9" s="2" t="s">
+    <row r="9" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="10" t="s">
+      <c r="D9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K9" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="L9" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" s="2" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A10" s="2" t="s">
+    <row r="10" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="2" t="s">
+      <c r="I10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="K10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="L10" s="6" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2069,10 +2052,10 @@
       <c r="C11" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G11" t="s">
@@ -2087,21 +2070,21 @@
       <c r="J11" t="s">
         <v>62</v>
       </c>
-      <c r="K11" s="6" t="s">
+      <c r="K11" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" ht="20" customHeight="1" spans="1:12">
-      <c r="A12" s="7" t="s">
+    <row r="12" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A12" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>44438</v>
       </c>
       <c r="D12" s="6" t="s">
@@ -2133,778 +2116,778 @@
       </c>
     </row>
     <row r="13" ht="20" customHeight="1" spans="1:12">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="D13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="J13" s="6" t="s">
+      <c r="G13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="K13" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="L13" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1" spans="1:12">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="J14" s="6" t="s">
+      <c r="G14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="K14" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="L14" s="6" t="s">
+      <c r="L14" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="15" s="2" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A15" s="9" t="s">
+    <row r="15" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A15" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="10" t="s">
+      <c r="B15" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="10" t="s">
+      <c r="D15" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="J15" s="10" t="s">
+      <c r="G15" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J15" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="K15" s="10" t="s">
+      <c r="K15" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="L15" s="10" t="s">
+      <c r="L15" s="6" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1" spans="1:12">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="J16" s="6" t="s">
+      <c r="G16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="K16" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="L16" s="6" t="s">
+      <c r="L16" s="4" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1" spans="1:12">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="6" t="s">
+      <c r="D17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="J17" s="6" t="s">
+      <c r="G17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="K17" s="6" t="s">
+      <c r="K17" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="L17" s="6" t="s">
+      <c r="L17" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1" spans="1:12">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="B18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="6" t="s">
+      <c r="D18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="J18" s="6" t="s">
+      <c r="G18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="K18" s="6" t="s">
+      <c r="K18" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="L18" s="6" t="s">
+      <c r="L18" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="19" s="2" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A19" s="9" t="s">
+    <row r="19" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A19" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G19" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="I19" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="J19" s="10" t="s">
+      <c r="G19" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="K19" s="10" t="s">
+      <c r="K19" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="L19" s="10" t="s">
+      <c r="L19" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="20" s="2" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A20" s="9" t="s">
+    <row r="20" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A20" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G20" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="J20" s="10" t="s">
+      <c r="G20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J20" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="K20" s="10" t="s">
+      <c r="K20" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="L20" s="10" t="s">
+      <c r="L20" s="6" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1" spans="1:12">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H21" s="6" t="s">
+      <c r="G21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="J21" s="6" t="s">
+      <c r="I21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J21" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="K21" s="6" t="s">
+      <c r="K21" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="L21" s="6" t="s">
+      <c r="L21" s="4" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1" spans="1:12">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6" t="s">
+      <c r="D22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="J22" s="6" t="s">
+      <c r="J22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K22" s="6" t="s">
+      <c r="K22" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="L22" s="6" t="s">
+      <c r="L22" s="4" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1" spans="1:12">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="B23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="G23" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="20">
+      <c r="G23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="17">
         <v>0.53</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="J23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6" t="s">
+      <c r="K23" s="4"/>
+      <c r="L23" s="4" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1" spans="1:12">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="B24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="6" t="s">
+      <c r="D24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="6" t="s">
+      <c r="G24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="I24" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="J24" s="6" t="s">
+      <c r="J24" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K24" s="6" t="s">
+      <c r="K24" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="L24" s="6" t="s">
+      <c r="L24" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="25" s="2" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A25" s="10" t="s">
+    <row r="25" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A25" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="H25" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="10" t="s">
+      <c r="H25" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="J25" s="10" t="s">
+      <c r="J25" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K25" s="10" t="s">
+      <c r="K25" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="L25" s="10" t="s">
+      <c r="L25" s="6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="26" s="2" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A26" s="10" t="s">
+    <row r="26" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A26" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="G26" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I26" s="10" t="s">
+      <c r="G26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="J26" s="10" t="s">
+      <c r="J26" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K26" s="10" t="s">
+      <c r="K26" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="L26" s="10" t="s">
+      <c r="L26" s="6" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="27" s="2" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A27" s="10" t="s">
+    <row r="27" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A27" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10" t="s">
+      <c r="E27" s="6"/>
+      <c r="F27" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="G27" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="10" t="s">
+      <c r="G27" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="J27" s="10" t="s">
+      <c r="J27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K27" s="10" t="s">
+      <c r="K27" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="L27" s="10" t="s">
+      <c r="L27" s="6" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1" spans="1:12">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="6" t="s">
+      <c r="B28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28" s="6" t="s">
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="J28" s="6" t="s">
+      <c r="J28" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K28" s="6" t="s">
+      <c r="K28" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="L28" s="6" t="s">
+      <c r="L28" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="29" s="2" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A29" s="10" t="s">
+    <row r="29" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A29" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="10" t="s">
+      <c r="B29" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10" t="s">
+      <c r="E29" s="6"/>
+      <c r="F29" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="G29" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I29" s="10" t="s">
+      <c r="G29" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="J29" s="10" t="s">
+      <c r="J29" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K29" s="10" t="s">
+      <c r="K29" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="L29" s="10" t="s">
+      <c r="L29" s="6" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1" spans="1:12">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6" t="s">
+      <c r="E30" s="4"/>
+      <c r="F30" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="G30" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="6" t="s">
+      <c r="G30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="J30" s="6" t="s">
+      <c r="J30" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K30" s="6" t="s">
+      <c r="K30" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="L30" s="6" t="s">
+      <c r="L30" s="4" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1" spans="1:12">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="B31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6" t="s">
+      <c r="D31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="G31" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="6" t="s">
+      <c r="G31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="J31" s="6" t="s">
+      <c r="J31" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K31" s="6" t="s">
+      <c r="K31" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="L31" s="6" t="s">
+      <c r="L31" s="4" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1" spans="1:12">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="6" t="s">
+      <c r="B32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6" t="s">
+      <c r="E32" s="4"/>
+      <c r="F32" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="G32" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I32" s="6" t="s">
+      <c r="G32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="J32" s="6" t="s">
+      <c r="J32" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K32" s="6" t="s">
+      <c r="K32" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="L32" s="6" t="s">
+      <c r="L32" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="33" s="2" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A33" s="10" t="s">
+    <row r="33" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A33" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B33" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="10" t="s">
+      <c r="B33" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I33" s="10" t="s">
+      <c r="D33" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="J33" s="10" t="s">
+      <c r="J33" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K33" s="10" t="s">
+      <c r="K33" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="L33" s="10" t="s">
+      <c r="L33" s="6" t="s">
         <v>173</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correciones de colores y ortografía
</commit_message>
<xml_diff>
--- a/Resources/data/COMPILADO DE  ENTIDADES FEDERATIVAS.xlsx
+++ b/Resources/data/COMPILADO DE  ENTIDADES FEDERATIVAS.xlsx
@@ -202,6 +202,9 @@
     <t>Durango</t>
   </si>
   <si>
+    <t>Por definir</t>
+  </si>
+  <si>
     <t>La Secretaría de Educación del Estado de Durango (SEED), todavía no tiene definido si el regreso a clases será presencial, virtual o híbrido, primero podría darse a conocer el calendario escolar.</t>
   </si>
   <si>
@@ -281,9 +284,6 @@
   </si>
   <si>
     <t>Hidalgo</t>
-  </si>
-  <si>
-    <t>Por definir</t>
   </si>
   <si>
     <t>**Solicitan postergar, fecha no definida</t>
@@ -825,7 +825,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -835,12 +835,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1161,139 +1155,139 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1306,23 +1300,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1335,11 +1325,7 @@
     <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1673,9 +1659,9 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1691,40 +1677,40 @@
   </cols>
   <sheetData>
     <row r="1" ht="71.25" spans="1:12">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1741,10 +1727,10 @@
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -1759,10 +1745,10 @@
       <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1779,10 +1765,10 @@
       <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -1797,10 +1783,10 @@
       <c r="J3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="4" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1817,45 +1803,45 @@
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" s="2" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A5" s="2" t="s">
+    <row r="5" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="2" t="s">
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1884,10 +1870,10 @@
       <c r="J6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1904,10 +1890,10 @@
       <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="4" t="s">
         <v>45</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1922,10 +1908,10 @@
       <c r="J7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="K7" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="4" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1942,7 +1928,7 @@
       <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -1960,10 +1946,10 @@
       <c r="J8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1980,7 +1966,7 @@
       <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -1998,10 +1984,10 @@
       <c r="J9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="L9" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2010,16 +1996,16 @@
         <v>56</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>57</v>
+      <c r="E10" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>50</v>
@@ -2036,16 +2022,16 @@
       <c r="J10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="K10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="L10" s="7" t="s">
-        <v>58</v>
+      <c r="L10" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
       <c r="A11" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>22</v>
@@ -2053,11 +2039,11 @@
       <c r="C11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="7" t="s">
+      <c r="E11" s="11" t="s">
         <v>61</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>13</v>
@@ -2069,826 +2055,826 @@
         <v>17</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K11" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="K11" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="L11" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="12" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A12" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="8">
+      <c r="B12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="6">
         <v>44438</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="7" t="s">
+      <c r="D12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J12" s="7" t="s">
+      <c r="F12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="G12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="K12" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="L12" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="13" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A13" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="D13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="K13" s="7" t="s">
+      <c r="F13" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="G13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>77</v>
       </c>
+      <c r="L13" s="4" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="14" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A14" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="B14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="K14" s="7" t="s">
+      <c r="G14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="L14" s="7" t="s">
+      <c r="L14" s="4" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="7" t="s">
+      <c r="D15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="K15" s="7" t="s">
+      <c r="G15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="L15" s="4" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" s="7" t="s">
+      <c r="B16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="K16" s="7" t="s">
+      <c r="G16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="L16" s="7" t="s">
+      <c r="L16" s="4" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="B17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="7" t="s">
+      <c r="D17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="G17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="K17" s="7" t="s">
+      <c r="G17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K17" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="L17" s="7" t="s">
+      <c r="L17" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="B18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="7" t="s">
+      <c r="D18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="G18" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="K18" s="7" t="s">
+      <c r="G18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K18" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="L18" s="7" t="s">
+      <c r="L18" s="4" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="10" t="s">
+      <c r="B19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="K19" s="7" t="s">
+      <c r="G19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K19" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="L19" s="7" t="s">
+      <c r="L19" s="4" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="11" t="s">
+      <c r="B20" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="K20" s="7" t="s">
+      <c r="G20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K20" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="L20" s="7" t="s">
+      <c r="L20" s="4" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="11" t="s">
+      <c r="B21" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H21" s="7" t="s">
+      <c r="G21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="K21" s="7" t="s">
+      <c r="I21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K21" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="L21" s="7" t="s">
+      <c r="L21" s="4" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="B22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7" t="s">
+      <c r="D22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="H22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="I22" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="J22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K22" s="7" t="s">
+      <c r="K22" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="L22" s="7" t="s">
+      <c r="L22" s="4" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="7" t="s">
+      <c r="B23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="17">
+      <c r="G23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="13">
         <v>0.53</v>
       </c>
-      <c r="J23" s="7" t="s">
+      <c r="J23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7" t="s">
+      <c r="K23" s="4"/>
+      <c r="L23" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="24" ht="20" customHeight="1" spans="1:12">
-      <c r="A24" s="12" t="s">
+    <row r="24" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A24" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="12" t="s">
+      <c r="B24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="12" t="s">
+      <c r="D24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="G24" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="12" t="s">
+      <c r="G24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I24" s="12" t="s">
+      <c r="I24" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="J24" s="12" t="s">
+      <c r="J24" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K24" s="12" t="s">
+      <c r="K24" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="L24" s="12" t="s">
+      <c r="L24" s="4" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="E25" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A26" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D26" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F25" s="7" t="s">
+      <c r="G26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A27" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="C27" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="H25" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="7" t="s">
+      <c r="E27" s="4"/>
+      <c r="F27" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="J25" s="7" t="s">
+      <c r="J27" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K25" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="L25" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A26" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="B26" s="7" t="s">
+      <c r="K27" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A28" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A29" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A30" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="F26" s="7" t="s">
+      <c r="D30" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="G26" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I26" s="7" t="s">
+      <c r="E30" s="4"/>
+      <c r="F30" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="J26" s="7" t="s">
+      <c r="J30" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K26" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="L26" s="7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="27" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A27" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="B27" s="7" t="s">
+      <c r="K30" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A31" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A32" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="7" t="s">
+      <c r="E32" s="4"/>
+      <c r="F32" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="J27" s="7" t="s">
+      <c r="J32" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K27" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="L27" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="28" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A28" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28" s="7" t="s">
+      <c r="K32" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A33" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="J28" s="7" t="s">
+      <c r="J33" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K28" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="L28" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="29" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A29" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="L29" s="7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="30" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A30" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K30" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="L30" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="31" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A31" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K31" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L31" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="32" ht="20" customHeight="1" spans="1:12">
-      <c r="A32" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K32" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="L32" s="12" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="33" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A33" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K33" s="7" t="s">
+      <c r="K33" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="L33" s="7" t="s">
+      <c r="L33" s="4" t="s">
         <v>173</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se agregaron las referencias consultadas para la información
</commit_message>
<xml_diff>
--- a/Resources/data/COMPILADO DE  ENTIDADES FEDERATIVAS.xlsx
+++ b/Resources/data/COMPILADO DE  ENTIDADES FEDERATIVAS.xlsx
@@ -331,11 +331,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.jalisco.gob.mx/es/prensa/noticias/129538
+    <t>https://www.jalisco.gob.mx/es/prensa/noticias/129538
 https://www.jalisco.gob.mx/es/prensa/noticias/127052
 https://www.facebook.com/educacion.jalisco/photos/a.446164440747/10158547049890748/
-https://portalsej.jalisco.gob.mx/plan-jalisco-para-la-reactivacion-economica/
-</t>
+https://portalsej.jalisco.gob.mx/plan-jalisco-para-la-reactivacion-economica/</t>
   </si>
   <si>
     <t>México</t>
@@ -635,16 +634,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
-    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
-    <numFmt numFmtId="177" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="176" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="177" formatCode="##"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="mmm\-yy"/>
+    <numFmt numFmtId="178" formatCode="dd\-mmm"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="##"/>
+    <numFmt numFmtId="179" formatCode="mmm\-yy"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -683,9 +682,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -697,17 +696,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -720,7 +711,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -736,7 +727,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -750,6 +772,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -759,22 +782,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -795,37 +803,21 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -840,31 +832,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -876,157 +1018,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1051,30 +1049,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1112,6 +1086,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1123,6 +1106,32 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1141,200 +1150,206 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="48" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1658,10 +1673,10 @@
   <sheetPr/>
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1677,136 +1692,136 @@
   </cols>
   <sheetData>
     <row r="1" ht="71.25" spans="1:12">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A4" s="1" t="s">
+    <row r="4" s="2" customFormat="1" ht="20" customHeight="1" spans="1:12">
+      <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="7" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1814,19 +1829,19 @@
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="16" t="s">
         <v>35</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -1841,77 +1856,79 @@
       <c r="J5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="G7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="19" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1928,7 +1945,7 @@
       <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -1946,86 +1963,86 @@
       <c r="J8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="D9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="I10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="19" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2039,10 +2056,10 @@
       <c r="C11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="5" t="s">
         <v>62</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -2057,828 +2074,840 @@
       <c r="J11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="6">
+      <c r="B12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="8">
         <v>44438</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="D12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J12" s="4" t="s">
+      <c r="G12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="7" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="4" t="s">
+      <c r="D13" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J13" s="4" t="s">
+      <c r="G13" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J14" s="4" t="s">
+      <c r="G14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="7" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="D15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J15" s="4" t="s">
+      <c r="G15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="L15" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J16" s="4" t="s">
+      <c r="G16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="L16" s="5" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="4" t="s">
+      <c r="D17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J17" s="4" t="s">
+      <c r="G17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="L17" s="7" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="D18" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J18" s="4" t="s">
+      <c r="G18" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="L18" s="5" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J19" s="4" t="s">
+      <c r="G19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="L19" s="19" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J20" s="4" t="s">
+      <c r="G20" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="L20" s="4" t="s">
+      <c r="L20" s="7" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H21" s="4" t="s">
+      <c r="G21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J21" s="4" t="s">
+      <c r="I21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="L21" s="4" t="s">
+      <c r="L21" s="5" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="B22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4" t="s">
+      <c r="D22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I22" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J22" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="L22" s="4" t="s">
+      <c r="L22" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="B23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="13">
+      <c r="G23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="20">
         <v>0.53</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4" t="s">
+      <c r="K23" s="7"/>
+      <c r="L23" s="19" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="24" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="B24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="4" t="s">
+      <c r="D24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="4" t="s">
+      <c r="G24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="I24" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="J24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="K24" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="L24" s="4" t="s">
+      <c r="L24" s="5" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="H25" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="4" t="s">
+      <c r="H25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="J25" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="K25" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="L25" s="4" t="s">
+      <c r="L25" s="19" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="26" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I26" s="4" t="s">
+      <c r="G26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J26" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="K26" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="L26" s="4" t="s">
+      <c r="L26" s="19" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4" t="s">
+      <c r="E27" s="7"/>
+      <c r="F27" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G27" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="4" t="s">
+      <c r="G27" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J27" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="K27" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="L27" s="4" t="s">
+      <c r="L27" s="7" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="B28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28" s="4" t="s">
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="J28" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="K28" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="L28" s="4" t="s">
+      <c r="L28" s="5" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="4" t="s">
+      <c r="B29" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4" t="s">
+      <c r="E29" s="7"/>
+      <c r="F29" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="G29" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I29" s="4" t="s">
+      <c r="G29" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="J29" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="K29" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="L29" s="4" t="s">
+      <c r="L29" s="19" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="B30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4" t="s">
+      <c r="E30" s="5"/>
+      <c r="F30" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="G30" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="4" t="s">
+      <c r="G30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="J30" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K30" s="4" t="s">
+      <c r="K30" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="L30" s="4" t="s">
+      <c r="L30" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="B31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4" t="s">
+      <c r="D31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="G31" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="4" t="s">
+      <c r="G31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="J31" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="K31" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="L31" s="4" t="s">
+      <c r="L31" s="19" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="32" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="B32" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4" t="s">
+      <c r="E32" s="5"/>
+      <c r="F32" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="G32" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I32" s="4" t="s">
+      <c r="G32" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="J32" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="K32" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="L32" s="4" t="s">
+      <c r="L32" s="5" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="33" s="1" customFormat="1" ht="20" customHeight="1" spans="1:12">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I33" s="4" t="s">
+      <c r="D33" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="J33" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="K33" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="L33" s="4" t="s">
+      <c r="L33" s="19" t="s">
         <v>173</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L9" r:id="rId1" display="http://www.chihuahua.gob.mx/contenidos/podemos-pensar-en-regreso-clases-presenciales-el-proximo-ciclo-javier-corral"/>
+    <hyperlink ref="L29" r:id="rId2" display="https://www.tamaulipas.gob.mx/educacion/avisos/planteles-seleccionados-fase-2/"/>
+    <hyperlink ref="L26" r:id="rId3" display="https://mieducacion.sepyc.gob.mx/sinaloa-coincide-con-el-presidente-andres-manuel-lopez-obrador-el-regreso-a-clases-es-por-el-convencimiento-nada-por-la-fuerza/"/>
+    <hyperlink ref="L10" r:id="rId4" display="https://www.elsiglodedurango.com.mx/2021/07/1329808.modelo-de-regreso-a-clases-sigue-sin-ser-definido-seed.html"/>
+    <hyperlink ref="L33" r:id="rId5" display="http://www.seduzac.gob.mx/portal/index.php"/>
+    <hyperlink ref="L25" r:id="rId6" display="https://slp.gob.mx/sege/Paginas/NOTICIAS/FECHAS-Y-MODALIDAD-DE-REGRESO-A-CLASES--SE-DAR%C3%81N-A-CONOCER-LA-PR%C3%93XIMA-SEMANA.aspx"/>
+    <hyperlink ref="L19" r:id="rId7" display="https://www.nayarit.gob.mx/seccion/educacion"/>
+    <hyperlink ref="L23" r:id="rId8" display="https://queretaro.gob.mx/regresoaclaseguro.aspx"/>
+    <hyperlink ref="L7" r:id="rId9" display="https://seceduccol-my.sharepoint.com/personal/publicaciones_web_secolima_gob_mx/_layouts/15/onedrive.aspx?id=%2Fpersonal%2Fpublicaciones%5Fweb%5Fsecolima%5Fgob%5Fmx%2FDocuments%2FPublicaciones%2FOtros%2F2021%2FPrueba%20Piloto%20de%20Asesori%CC%81a%20Aca%CC%81demicas%20y%20Apoyo%20Socioemocional%2Epdf&amp;parent=%2Fpersonal%2Fpublicaciones%5Fweb%5Fsecolima%5Fgob%5Fmx%2FDocuments%2FPublicaciones%2FOtros%2F2021&amp;originalPath=aHR0cHM6Ly9zZWNlZHVjY29sLW15LnNoYXJlcG9pbnQuY29tLzpiOi9nL3BlcnNvbmFsL3B1YmxpY2FjaW9uZXNfd2ViX3NlY29saW1hX2dvYl9teC9FUldlQjVMalQ4MUdud1FkUnNqZC0wb0I3SHI3RjlTcG5idldYWlhUSzJINkR3P3J0aW1lPUozS09XQjVWMlVn"/>
+    <hyperlink ref="L31" r:id="rId10" display="https://www.sev.gob.mx/v1/noticias/leer/2354/"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>

</xml_diff>